<commit_message>
Cambio de nombres de los archivos
</commit_message>
<xml_diff>
--- a/trunk/requirements/documentation/Support/Estimacion Marco.xlsx
+++ b/trunk/requirements/documentation/Support/Estimacion Marco.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="18915" windowHeight="8475"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="103">
   <si>
     <t>Modificar fecha de inicio y fin de un trabajo.</t>
   </si>
@@ -315,9 +315,6 @@
   </si>
   <si>
     <t>Semanas de SPRINT</t>
-  </si>
-  <si>
-    <t>v</t>
   </si>
   <si>
     <t>Total semanas ideales</t>
@@ -332,8 +329,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,12 +528,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
-    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
-    <cellStyle name="Accent5" xfId="4" builtinId="45"/>
+    <cellStyle name="60% - Énfasis5" xfId="5" builtinId="48"/>
+    <cellStyle name="Énfasis1" xfId="3" builtinId="29"/>
+    <cellStyle name="Énfasis5" xfId="4" builtinId="45"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="2" builtinId="10"/>
+    <cellStyle name="Notas" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -555,7 +552,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -629,7 +626,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -664,7 +660,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -840,14 +835,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -860,7 +855,7 @@
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1">
       <c r="A1" s="23" t="s">
         <v>86</v>
       </c>
@@ -873,7 +868,7 @@
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
@@ -898,7 +893,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -923,7 +918,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -948,7 +943,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -973,7 +968,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -993,7 +988,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1019,7 +1014,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1044,7 +1039,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1070,7 +1065,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1090,7 +1085,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1116,7 +1111,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1142,7 +1137,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1162,7 +1157,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15.75" thickBot="1">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1179,7 +1174,7 @@
         <v>3</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I15" s="11">
         <f>I13/I12</f>
@@ -1188,7 +1183,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15.75" thickBot="1">
       <c r="C16" s="5"/>
       <c r="D16" s="10" t="s">
         <v>78</v>
@@ -1204,12 +1199,12 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="C17" s="5"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
@@ -1233,7 +1228,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1258,7 +1253,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1275,7 +1270,7 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I20" s="3">
         <f>I15</f>
@@ -1284,7 +1279,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1304,7 +1299,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1321,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I22" s="11">
         <f>I20/I19</f>
@@ -1330,7 +1325,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1350,7 +1345,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1369,7 +1364,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1392,7 +1387,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1417,7 +1412,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1442,7 +1437,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1467,7 +1462,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -1492,7 +1487,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="15.75" thickBot="1">
       <c r="D30" s="10" t="s">
         <v>79</v>
       </c>
@@ -1513,7 +1508,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="C31" s="5"/>
       <c r="H31" t="s">
         <v>57</v>
@@ -1524,7 +1519,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" s="7" t="s">
         <v>28</v>
       </c>
@@ -1550,7 +1545,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -1575,7 +1570,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1600,7 +1595,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1625,7 +1620,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="15.75" thickBot="1">
       <c r="C36" s="5"/>
       <c r="D36" s="10" t="s">
         <v>81</v>
@@ -1647,7 +1642,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="15.75" thickBot="1">
       <c r="C37" s="5"/>
       <c r="H37" s="16" t="s">
         <v>27</v>
@@ -1659,7 +1654,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" s="7" t="s">
         <v>28</v>
       </c>
@@ -1679,7 +1674,7 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -1698,7 +1693,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -1717,7 +1712,7 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="15.75" thickBot="1">
       <c r="C41" s="5"/>
       <c r="D41" s="10" t="s">
         <v>84</v>
@@ -1733,13 +1728,13 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="15.75" thickBot="1">
       <c r="C43" s="5"/>
       <c r="D43" s="12" t="s">
         <v>27</v>
@@ -1755,11 +1750,11 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" s="22" t="s">
         <v>16</v>
       </c>
@@ -1771,7 +1766,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" s="22" t="s">
         <v>18</v>
       </c>
@@ -1783,724 +1778,721 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="12:13">
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="12:13">
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="12:13">
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="12:13">
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="12:13">
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="12:13">
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="12:13">
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="12:13">
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="12:13">
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="12:13">
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H59" t="s">
-        <v>100</v>
-      </c>
+    <row r="59" spans="12:13">
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="12:13">
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="12:13">
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="12:13">
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="12:13">
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="12:13">
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="12:13">
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="12:13">
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="12:13">
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="12:13">
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="12:13">
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="12:13">
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="12:13">
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="12:13">
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="12:13">
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="12:13">
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="12:13">
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="12:13">
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
     </row>
-    <row r="77" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="12:13">
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="12:13">
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="12:13">
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="12:13">
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
     </row>
-    <row r="81" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="12:13">
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="12:13">
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
     </row>
-    <row r="83" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="12:13">
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
     </row>
-    <row r="84" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="12:13">
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
     </row>
-    <row r="85" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="12:13">
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
     </row>
-    <row r="86" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="12:13">
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
     </row>
-    <row r="87" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="12:13">
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
     </row>
-    <row r="88" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="12:13">
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
     </row>
-    <row r="89" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="12:13">
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
     </row>
-    <row r="90" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="12:13">
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
     </row>
-    <row r="91" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="12:13">
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
     </row>
-    <row r="92" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="12:13">
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
     </row>
-    <row r="93" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="12:13">
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
     </row>
-    <row r="94" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="12:13">
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
     </row>
-    <row r="95" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="12:13">
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
     </row>
-    <row r="96" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="12:13">
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
     </row>
-    <row r="97" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="12:13">
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
     </row>
-    <row r="98" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="12:13">
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
     </row>
-    <row r="99" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="12:13">
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
     </row>
-    <row r="100" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="12:13">
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
     </row>
-    <row r="101" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="12:13">
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
     </row>
-    <row r="102" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="12:13">
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
     </row>
-    <row r="103" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="12:13">
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
     </row>
-    <row r="104" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="12:13">
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
     </row>
-    <row r="105" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="12:13">
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
     </row>
-    <row r="106" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="12:13">
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
     </row>
-    <row r="107" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="12:13">
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
     </row>
-    <row r="108" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="12:13">
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
     </row>
-    <row r="109" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="12:13">
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
     </row>
-    <row r="110" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="12:13">
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
     </row>
-    <row r="111" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="12:13">
       <c r="L111" s="1"/>
       <c r="M111" s="1"/>
     </row>
-    <row r="112" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="12:13">
       <c r="L112" s="1"/>
       <c r="M112" s="1"/>
     </row>
-    <row r="113" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="12:13">
       <c r="L113" s="1"/>
       <c r="M113" s="1"/>
     </row>
-    <row r="114" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="12:13">
       <c r="L114" s="1"/>
       <c r="M114" s="1"/>
     </row>
-    <row r="115" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="12:13">
       <c r="L115" s="1"/>
       <c r="M115" s="1"/>
     </row>
-    <row r="116" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="12:13">
       <c r="L116" s="1"/>
       <c r="M116" s="1"/>
     </row>
-    <row r="117" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="12:13">
       <c r="L117" s="1"/>
       <c r="M117" s="1"/>
     </row>
-    <row r="118" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="12:13">
       <c r="L118" s="1"/>
       <c r="M118" s="1"/>
     </row>
-    <row r="119" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="12:13">
       <c r="L119" s="1"/>
       <c r="M119" s="1"/>
     </row>
-    <row r="120" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="12:13">
       <c r="L120" s="1"/>
       <c r="M120" s="1"/>
     </row>
-    <row r="121" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="12:13">
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
     </row>
-    <row r="122" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="12:13">
       <c r="L122" s="1"/>
       <c r="M122" s="1"/>
     </row>
-    <row r="123" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="12:13">
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
     </row>
-    <row r="124" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="12:13">
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
     </row>
-    <row r="125" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="12:13">
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
     </row>
-    <row r="126" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="12:13">
       <c r="L126" s="1"/>
       <c r="M126" s="1"/>
     </row>
-    <row r="127" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="12:13">
       <c r="L127" s="1"/>
       <c r="M127" s="1"/>
     </row>
-    <row r="128" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="12:13">
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
     </row>
-    <row r="129" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="12:13">
       <c r="L129" s="1"/>
       <c r="M129" s="1"/>
     </row>
-    <row r="130" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="12:13">
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
     </row>
-    <row r="131" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="12:13">
       <c r="L131" s="1"/>
       <c r="M131" s="1"/>
     </row>
-    <row r="132" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="12:13">
       <c r="L132" s="1"/>
       <c r="M132" s="1"/>
     </row>
-    <row r="133" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="12:13">
       <c r="L133" s="1"/>
       <c r="M133" s="1"/>
     </row>
-    <row r="134" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="12:13">
       <c r="L134" s="1"/>
       <c r="M134" s="1"/>
     </row>
-    <row r="135" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="12:13">
       <c r="L135" s="1"/>
       <c r="M135" s="1"/>
     </row>
-    <row r="136" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="12:13">
       <c r="L136" s="1"/>
       <c r="M136" s="1"/>
     </row>
-    <row r="137" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="12:13">
       <c r="L137" s="1"/>
       <c r="M137" s="1"/>
     </row>
-    <row r="138" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="12:13">
       <c r="L138" s="1"/>
       <c r="M138" s="1"/>
     </row>
-    <row r="139" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="12:13">
       <c r="L139" s="1"/>
       <c r="M139" s="1"/>
     </row>
-    <row r="140" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="12:13">
       <c r="L140" s="1"/>
       <c r="M140" s="1"/>
     </row>
-    <row r="141" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="12:13">
       <c r="L141" s="1"/>
       <c r="M141" s="1"/>
     </row>
-    <row r="142" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="12:13">
       <c r="L142" s="1"/>
       <c r="M142" s="1"/>
     </row>
-    <row r="143" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="12:13">
       <c r="L143" s="1"/>
       <c r="M143" s="1"/>
     </row>
-    <row r="144" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="12:13">
       <c r="L144" s="1"/>
       <c r="M144" s="1"/>
     </row>
-    <row r="145" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="12:13">
       <c r="L145" s="1"/>
       <c r="M145" s="1"/>
     </row>
-    <row r="146" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="12:13">
       <c r="L146" s="1"/>
       <c r="M146" s="1"/>
     </row>
-    <row r="147" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="12:13">
       <c r="L147" s="1"/>
       <c r="M147" s="1"/>
     </row>
-    <row r="148" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="12:13">
       <c r="L148" s="1"/>
       <c r="M148" s="1"/>
     </row>
-    <row r="149" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="12:13">
       <c r="L149" s="1"/>
       <c r="M149" s="1"/>
     </row>
-    <row r="150" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="12:13">
       <c r="L150" s="1"/>
       <c r="M150" s="1"/>
     </row>
-    <row r="151" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="12:13">
       <c r="L151" s="1"/>
       <c r="M151" s="1"/>
     </row>
-    <row r="152" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="12:13">
       <c r="L152" s="1"/>
       <c r="M152" s="1"/>
     </row>
-    <row r="153" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="12:13">
       <c r="L153" s="1"/>
       <c r="M153" s="1"/>
     </row>
-    <row r="154" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="12:13">
       <c r="L154" s="1"/>
       <c r="M154" s="1"/>
     </row>
-    <row r="155" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="12:13">
       <c r="L155" s="1"/>
       <c r="M155" s="1"/>
     </row>
-    <row r="156" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="12:13">
       <c r="L156" s="1"/>
       <c r="M156" s="1"/>
     </row>
-    <row r="157" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="12:13">
       <c r="L157" s="1"/>
       <c r="M157" s="1"/>
     </row>
-    <row r="158" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="12:13">
       <c r="L158" s="1"/>
       <c r="M158" s="1"/>
     </row>
-    <row r="159" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="12:13">
       <c r="L159" s="1"/>
       <c r="M159" s="1"/>
     </row>
-    <row r="160" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="12:13">
       <c r="L160" s="1"/>
       <c r="M160" s="1"/>
     </row>
-    <row r="161" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="12:13">
       <c r="L161" s="1"/>
       <c r="M161" s="1"/>
     </row>
-    <row r="162" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="12:13">
       <c r="L162" s="1"/>
       <c r="M162" s="1"/>
     </row>
-    <row r="163" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="12:13">
       <c r="L163" s="1"/>
       <c r="M163" s="1"/>
     </row>
-    <row r="164" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="12:13">
       <c r="L164" s="1"/>
       <c r="M164" s="1"/>
     </row>
-    <row r="165" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="12:13">
       <c r="L165" s="1"/>
       <c r="M165" s="1"/>
     </row>
-    <row r="166" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="12:13">
       <c r="L166" s="1"/>
       <c r="M166" s="1"/>
     </row>
-    <row r="167" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="12:13">
       <c r="L167" s="1"/>
       <c r="M167" s="1"/>
     </row>
-    <row r="168" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="12:13">
       <c r="L168" s="1"/>
       <c r="M168" s="1"/>
     </row>
-    <row r="169" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="12:13">
       <c r="L169" s="1"/>
       <c r="M169" s="1"/>
     </row>
-    <row r="170" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="12:13">
       <c r="L170" s="1"/>
       <c r="M170" s="1"/>
     </row>
-    <row r="171" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="12:13">
       <c r="L171" s="1"/>
       <c r="M171" s="1"/>
     </row>
-    <row r="172" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="12:13">
       <c r="L172" s="1"/>
       <c r="M172" s="1"/>
     </row>
-    <row r="173" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="12:13">
       <c r="L173" s="1"/>
       <c r="M173" s="1"/>
     </row>
-    <row r="174" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="12:13">
       <c r="L174" s="1"/>
       <c r="M174" s="1"/>
     </row>
-    <row r="175" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="12:13">
       <c r="L175" s="1"/>
       <c r="M175" s="1"/>
     </row>
-    <row r="176" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="12:13">
       <c r="L176" s="1"/>
       <c r="M176" s="1"/>
     </row>
-    <row r="177" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="12:13">
       <c r="L177" s="1"/>
       <c r="M177" s="1"/>
     </row>
-    <row r="178" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="12:13">
       <c r="L178" s="1"/>
       <c r="M178" s="1"/>
     </row>
-    <row r="179" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="12:13">
       <c r="L179" s="1"/>
       <c r="M179" s="1"/>
     </row>
-    <row r="180" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="12:13">
       <c r="L180" s="1"/>
       <c r="M180" s="1"/>
     </row>
-    <row r="181" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="12:13">
       <c r="L181" s="1"/>
       <c r="M181" s="1"/>
     </row>
-    <row r="182" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="12:13">
       <c r="L182" s="1"/>
       <c r="M182" s="1"/>
     </row>
-    <row r="183" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="12:13">
       <c r="L183" s="1"/>
       <c r="M183" s="1"/>
     </row>
-    <row r="184" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="12:13">
       <c r="L184" s="1"/>
       <c r="M184" s="1"/>
     </row>
-    <row r="185" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="12:13">
       <c r="L185" s="1"/>
       <c r="M185" s="1"/>
     </row>
-    <row r="186" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="12:13">
       <c r="L186" s="1"/>
       <c r="M186" s="1"/>
     </row>
-    <row r="187" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="12:13">
       <c r="L187" s="1"/>
       <c r="M187" s="1"/>
     </row>
-    <row r="188" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="12:13">
       <c r="L188" s="1"/>
       <c r="M188" s="1"/>
     </row>
-    <row r="189" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="12:13">
       <c r="L189" s="1"/>
       <c r="M189" s="1"/>
     </row>
-    <row r="190" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="12:13">
       <c r="L190" s="1"/>
       <c r="M190" s="1"/>
     </row>
-    <row r="191" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="12:13">
       <c r="L191" s="1"/>
       <c r="M191" s="1"/>
     </row>
-    <row r="192" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="12:13">
       <c r="L192" s="1"/>
       <c r="M192" s="1"/>
     </row>
-    <row r="193" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="12:13">
       <c r="L193" s="1"/>
       <c r="M193" s="1"/>
     </row>
-    <row r="194" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="12:13">
       <c r="L194" s="1"/>
       <c r="M194" s="1"/>
     </row>
-    <row r="195" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="12:13">
       <c r="L195" s="1"/>
       <c r="M195" s="1"/>
     </row>
-    <row r="196" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="12:13">
       <c r="L196" s="1"/>
       <c r="M196" s="1"/>
     </row>
-    <row r="197" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="12:13">
       <c r="L197" s="1"/>
       <c r="M197" s="1"/>
     </row>
-    <row r="198" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="12:13">
       <c r="L198" s="1"/>
       <c r="M198" s="1"/>
     </row>
-    <row r="199" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="12:13">
       <c r="L199" s="1"/>
       <c r="M199" s="1"/>
     </row>
-    <row r="200" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="12:13">
       <c r="L200" s="1"/>
       <c r="M200" s="1"/>
     </row>
-    <row r="201" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="12:13">
       <c r="L201" s="1"/>
       <c r="M201" s="1"/>
     </row>
-    <row r="202" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="12:13">
       <c r="L202" s="1"/>
       <c r="M202" s="1"/>
     </row>
-    <row r="203" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="12:13">
       <c r="L203" s="1"/>
       <c r="M203" s="1"/>
     </row>
-    <row r="204" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="12:13">
       <c r="L204" s="1"/>
       <c r="M204" s="1"/>
     </row>
-    <row r="205" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="12:13">
       <c r="L205" s="1"/>
       <c r="M205" s="1"/>
     </row>
-    <row r="206" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="12:13">
       <c r="L206" s="1"/>
       <c r="M206" s="1"/>
     </row>
-    <row r="207" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="12:13">
       <c r="L207" s="1"/>
       <c r="M207" s="1"/>
     </row>
-    <row r="208" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="12:13">
       <c r="L208" s="1"/>
       <c r="M208" s="1"/>
     </row>
-    <row r="209" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="12:13">
       <c r="L209" s="1"/>
       <c r="M209" s="1"/>
     </row>
-    <row r="210" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="12:13">
       <c r="L210" s="1"/>
       <c r="M210" s="1"/>
     </row>
-    <row r="211" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="12:13">
       <c r="L211" s="1"/>
       <c r="M211" s="1"/>
     </row>
-    <row r="212" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="12:13">
       <c r="L212" s="1"/>
       <c r="M212" s="1"/>
     </row>
-    <row r="213" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="12:13">
       <c r="L213" s="1"/>
       <c r="M213" s="1"/>
     </row>
-    <row r="214" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="12:13">
       <c r="L214" s="1"/>
       <c r="M214" s="1"/>
     </row>
-    <row r="215" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="12:13">
       <c r="L215" s="1"/>
       <c r="M215" s="1"/>
     </row>
-    <row r="216" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="12:13">
       <c r="L216" s="1"/>
       <c r="M216" s="1"/>
     </row>
-    <row r="217" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="12:13">
       <c r="L217" s="1"/>
       <c r="M217" s="1"/>
     </row>
-    <row r="218" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="12:13">
       <c r="L218" s="1"/>
       <c r="M218" s="1"/>
     </row>
-    <row r="219" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="12:13">
       <c r="L219" s="1"/>
       <c r="M219" s="1"/>
     </row>
-    <row r="220" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="12:13">
       <c r="L220" s="1"/>
       <c r="M220" s="1"/>
     </row>
-    <row r="221" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="12:13">
       <c r="L221" s="1"/>
     </row>
-    <row r="222" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="12:13">
       <c r="L222" s="1"/>
     </row>
-    <row r="223" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="12:13">
       <c r="L223" s="1"/>
     </row>
-    <row r="224" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="12:13">
       <c r="L224" s="1"/>
     </row>
-    <row r="225" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="12:12">
       <c r="L225" s="1"/>
     </row>
-    <row r="226" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="12:12">
       <c r="L226" s="1"/>
     </row>
-    <row r="227" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="12:12">
       <c r="L227" s="1"/>
     </row>
   </sheetData>
@@ -2518,14 +2510,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -2535,7 +2527,7 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="24" t="s">
         <v>97</v>
       </c>
@@ -2546,11 +2538,11 @@
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
@@ -2571,7 +2563,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2593,7 +2585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2615,7 +2607,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -2637,7 +2629,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -2659,7 +2651,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -2681,7 +2673,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -2704,7 +2696,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -2727,7 +2719,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -2748,7 +2740,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2770,7 +2762,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2793,7 +2785,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2815,7 +2807,7 @@
         <v>40.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2837,7 +2829,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2859,7 +2851,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2881,7 +2873,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2903,7 +2895,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2925,7 +2917,7 @@
         <v>57.6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
@@ -2946,7 +2938,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2968,7 +2960,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2990,7 +2982,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -3012,7 +3004,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -3034,7 +3026,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3058,7 +3050,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -3082,7 +3074,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
@@ -3105,7 +3097,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -3129,7 +3121,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -3152,7 +3144,7 @@
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -3175,7 +3167,7 @@
       </c>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="7" t="s">
         <v>28</v>
       </c>
@@ -3197,7 +3189,7 @@
       </c>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -3220,7 +3212,7 @@
       </c>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -3243,7 +3235,7 @@
       </c>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -3266,7 +3258,7 @@
       </c>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -3288,7 +3280,7 @@
         <v>136.5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -3310,7 +3302,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -3332,7 +3324,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="7" t="s">
         <v>28</v>
       </c>
@@ -3353,7 +3345,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -3375,7 +3367,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -3398,7 +3390,7 @@
       </c>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -3421,7 +3413,7 @@
       </c>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="7" t="s">
         <v>28</v>
       </c>
@@ -3443,7 +3435,7 @@
       </c>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -3465,12 +3457,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15.75" thickBot="1">
       <c r="D45" s="19" t="s">
         <v>27</v>
       </c>
@@ -3486,7 +3478,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="22" t="s">
         <v>16</v>
       </c>
@@ -3497,7 +3489,7 @@
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>

</xml_diff>